<commit_message>
bugs with integration errors and nans if gamma<1 but otherwise working
</commit_message>
<xml_diff>
--- a/OUTPUT/data.xlsx
+++ b/OUTPUT/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="53">
   <si>
     <t>id</t>
   </si>
@@ -34,100 +34,133 @@
     <t>event</t>
   </si>
   <si>
+    <t>photon</t>
+  </si>
+  <si>
     <t>electron</t>
   </si>
   <si>
-    <t>photon</t>
-  </si>
-  <si>
     <t>positron</t>
   </si>
   <si>
     <t>[1. 2. 3.]</t>
   </si>
   <si>
-    <t>[397.69934526 889.48028181 613.03654191]</t>
-  </si>
-  <si>
-    <t>[ 14688.76788313 -22310.57313792  16739.64226626]</t>
-  </si>
-  <si>
-    <t>[ 14794.16069403 -21396.01529931  16858.57174596]</t>
-  </si>
-  <si>
-    <t>[ 24337.5782651  -20739.49993442  27218.19766623]</t>
-  </si>
-  <si>
-    <t>[ 24300.47364053 -20275.06582948  27177.91938526]</t>
-  </si>
-  <si>
-    <t>[ 16361.14238225 -23078.23907106  16462.20510208]</t>
-  </si>
-  <si>
-    <t>[ 15393.87880457 -23756.25351602  15152.31988992]</t>
-  </si>
-  <si>
-    <t>[ 662897.2133463    93985.83869198 1059912.27377766]</t>
-  </si>
-  <si>
-    <t>[ 16090.14002955 -23951.13242144  16260.04782948]</t>
+    <t>[24508.65269744 54829.56344934 37690.39192712]</t>
+  </si>
+  <si>
+    <t>[24721.6900838  54710.16577208 38017.80126594]</t>
+  </si>
+  <si>
+    <t>[19564.8616914  60960.697398   22414.95269621]</t>
+  </si>
+  <si>
+    <t>[24409.56940619 54367.19571873 37858.44258768]</t>
+  </si>
+  <si>
+    <t>[  68061.00739401 1978524.49768041  144460.66410187]</t>
+  </si>
+  <si>
+    <t>[24879.50262682 55037.40781384 38260.33757025]</t>
+  </si>
+  <si>
+    <t>[25091.74805529 56063.97503394 38494.77543305]</t>
+  </si>
+  <si>
+    <t>[29951.9990088  53916.93661228 55352.45522456]</t>
+  </si>
+  <si>
+    <t>[29882.1747087  54195.88760318 54772.39534386]</t>
+  </si>
+  <si>
+    <t>[5855021.16886212 7075783.29386117 5923060.75478291]</t>
+  </si>
+  <si>
+    <t>[25234.04265409 56481.83558126 38985.20191172]</t>
+  </si>
+  <si>
+    <t>[26247.57270091 56014.75837767 40742.74741594]</t>
+  </si>
+  <si>
+    <t>[58966.29564398 59287.41113592 78858.80599506]</t>
   </si>
   <si>
     <t>[15. 20.]</t>
   </si>
   <si>
-    <t>[1.08903415 6.01865234]</t>
-  </si>
-  <si>
-    <t>[1.08903363 5.26448506]</t>
-  </si>
-  <si>
-    <t>[1.08903247 4.82712197]</t>
-  </si>
-  <si>
-    <t>[ 1.08903247 -4.82712197]</t>
-  </si>
-  <si>
-    <t>[1.17117919 0.02262817]</t>
-  </si>
-  <si>
-    <t>[1.17118573 0.06868427]</t>
-  </si>
-  <si>
-    <t>[1.1711708  1.65051912]</t>
-  </si>
-  <si>
-    <t>[ 1.1711708  -1.65051912]</t>
-  </si>
-  <si>
-    <t>[0.83447708 1.42703275]</t>
-  </si>
-  <si>
-    <t>[0.83441756 3.48100358]</t>
-  </si>
-  <si>
-    <t>[0.83074485 3.75296357]</t>
-  </si>
-  <si>
-    <t>[ 0.83074485 -3.75296357]</t>
-  </si>
-  <si>
-    <t>[2.46190652 6.01027548]</t>
-  </si>
-  <si>
-    <t>[2.47315226 0.17987475]</t>
-  </si>
-  <si>
-    <t>[2.38211146 0.94127591]</t>
-  </si>
-  <si>
-    <t>[ 2.38211146 -0.94127591]</t>
-  </si>
-  <si>
-    <t>[0.47015929 3.77348094]</t>
-  </si>
-  <si>
-    <t>[0.4857604 4.2213964]</t>
+    <t>[14.99948899  5.77235136]</t>
+  </si>
+  <si>
+    <t>[14.99948899 -5.77235136]</t>
+  </si>
+  <si>
+    <t>[0.32081834 1.19405907]</t>
+  </si>
+  <si>
+    <t>[0.3368392  2.26060968]</t>
+  </si>
+  <si>
+    <t>[0.37241882 3.65593015]</t>
+  </si>
+  <si>
+    <t>[ 0.37241882 -3.65593015]</t>
+  </si>
+  <si>
+    <t>[0.33332945 2.54382368]</t>
+  </si>
+  <si>
+    <t>[0.42188361 1.54811421]</t>
+  </si>
+  <si>
+    <t>[0.23827808 0.30056747]</t>
+  </si>
+  <si>
+    <t>[ 0.23827808 -0.30056747]</t>
+  </si>
+  <si>
+    <t>[1.13217414 1.36691641]</t>
+  </si>
+  <si>
+    <t>[1.13164268 2.53692433]</t>
+  </si>
+  <si>
+    <t>[0.29437794 1.24258164]</t>
+  </si>
+  <si>
+    <t>[0.29246225 5.86720934]</t>
+  </si>
+  <si>
+    <t>[0.31658228 3.63343614]</t>
+  </si>
+  <si>
+    <t>[ 0.31658228 -3.63343614]</t>
+  </si>
+  <si>
+    <t>[1.38707495 2.00859345]</t>
+  </si>
+  <si>
+    <t>[1.44945382 0.87826284]</t>
+  </si>
+  <si>
+    <t>[ 1.70235239 -3.59269334]</t>
+  </si>
+  <si>
+    <t>[0.61465117 5.85135185]</t>
+  </si>
+  <si>
+    <t>[0.6168182  0.98620691]</t>
+  </si>
+  <si>
+    <t>[1.02290727 1.39072078]</t>
+  </si>
+  <si>
+    <t>[1.03213726 0.09969227]</t>
+  </si>
+  <si>
+    <t>[1.04152001 5.20777295]</t>
+  </si>
+  <si>
+    <t>[ 1.04152001 -5.20777295]</t>
   </si>
   <si>
     <t>PRIMARY</t>
@@ -136,10 +169,10 @@
     <t>MOVE</t>
   </si>
   <si>
+    <t>PAIR PRODUCTION</t>
+  </si>
+  <si>
     <t>BREMSSTRAHLUNG</t>
-  </si>
-  <si>
-    <t>PAIR PRODUCTION</t>
   </si>
 </sst>
 </file>
@@ -497,7 +530,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -528,22 +561,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2">
-        <v>1000000</v>
+        <v>1000</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -551,22 +584,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3">
-        <v>999989.0807026449</v>
+        <v>1000</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -574,22 +607,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4">
-        <v>562451.0813495668</v>
+        <v>34.19096534435106</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -597,22 +630,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5">
-        <v>437537.9993530781</v>
+        <v>965.8090346556489</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -626,16 +659,16 @@
         <v>7</v>
       </c>
       <c r="D6">
-        <v>437537.9993530781</v>
+        <v>31.89638555785016</v>
       </c>
       <c r="E6" t="s">
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -643,22 +676,22 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D7">
-        <v>359444.0453689487</v>
+        <v>17.5340151332472</v>
       </c>
       <c r="E7" t="s">
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -669,19 +702,19 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D8">
-        <v>78093.95398412942</v>
+        <v>14.36237042460295</v>
       </c>
       <c r="E8" t="s">
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G8" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -692,19 +725,19 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D9">
-        <v>78086.67849243502</v>
+        <v>14.36237042460295</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -712,22 +745,22 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10">
-        <v>43861.13810405511</v>
+        <v>5.805174018462141</v>
       </c>
       <c r="E10" t="s">
         <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G10" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -735,22 +768,22 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D11">
-        <v>34225.54038837991</v>
+        <v>8.557196406140813</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G11" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -758,22 +791,22 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
       </c>
       <c r="D12">
-        <v>34225.54038837991</v>
+        <v>5.770566295008839</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
       </c>
       <c r="F12" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G12" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -781,22 +814,22 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D13">
-        <v>8587.915142542295</v>
+        <v>2.987384164531072</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
       </c>
       <c r="F13" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G13" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -807,19 +840,19 @@
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D14">
-        <v>25637.62524583761</v>
+        <v>2.783182130477767</v>
       </c>
       <c r="E14" t="s">
         <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G14" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -827,22 +860,22 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
       </c>
       <c r="D15">
-        <v>8584.446832212987</v>
+        <v>2.783182130477767</v>
       </c>
       <c r="E15" t="s">
         <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G15" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -850,22 +883,22 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D16">
-        <v>8445.310316489044</v>
+        <v>1.724253354036095</v>
       </c>
       <c r="E16" t="s">
         <v>14</v>
       </c>
       <c r="F16" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G16" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -873,22 +906,22 @@
         <v>15</v>
       </c>
       <c r="B17">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
         <v>8</v>
       </c>
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
       <c r="D17">
-        <v>139.136515723943</v>
+        <v>1.058928776441672</v>
       </c>
       <c r="E17" t="s">
         <v>14</v>
       </c>
       <c r="F17" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G17" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -896,22 +929,22 @@
         <v>16</v>
       </c>
       <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
         <v>8</v>
       </c>
-      <c r="C18" t="s">
-        <v>7</v>
-      </c>
       <c r="D18">
-        <v>139.136515723943</v>
+        <v>961.5091125054774</v>
       </c>
       <c r="E18" t="s">
         <v>15</v>
       </c>
       <c r="F18" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G18" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -919,22 +952,22 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D19">
-        <v>55.38041740010019</v>
+        <v>274.1870826078945</v>
       </c>
       <c r="E19" t="s">
         <v>15</v>
       </c>
       <c r="F19" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G19" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -945,19 +978,19 @@
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D20">
-        <v>83.75609832384279</v>
+        <v>687.322029897583</v>
       </c>
       <c r="E20" t="s">
         <v>15</v>
       </c>
       <c r="F20" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G20" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -965,22 +998,22 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D21">
-        <v>45.4400991308176</v>
+        <v>266.7476377361234</v>
       </c>
       <c r="E21" t="s">
         <v>16</v>
       </c>
       <c r="F21" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G21" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -988,22 +1021,22 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D22">
-        <v>39.82714717113742</v>
+        <v>245.5616149816444</v>
       </c>
       <c r="E22" t="s">
         <v>16</v>
       </c>
       <c r="F22" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G22" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1014,19 +1047,19 @@
         <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D23">
-        <v>5.61295195968018</v>
+        <v>21.18602275447892</v>
       </c>
       <c r="E23" t="s">
         <v>16</v>
       </c>
       <c r="F23" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G23" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1037,19 +1070,19 @@
         <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D24">
-        <v>5.61295195968018</v>
+        <v>21.18602275447892</v>
       </c>
       <c r="E24" t="s">
         <v>17</v>
       </c>
       <c r="F24" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G24" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1060,19 +1093,19 @@
         <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D25">
-        <v>1.848704372651212</v>
+        <v>16.56019496691658</v>
       </c>
       <c r="E25" t="s">
         <v>17</v>
       </c>
       <c r="F25" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G25" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1086,16 +1119,16 @@
         <v>8</v>
       </c>
       <c r="D26">
-        <v>3.764247587028968</v>
+        <v>4.625827787562347</v>
       </c>
       <c r="E26" t="s">
         <v>17</v>
       </c>
       <c r="F26" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G26" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1103,22 +1136,22 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D27">
-        <v>32.75455495771459</v>
+        <v>8.191997847693441</v>
       </c>
       <c r="E27" t="s">
         <v>18</v>
       </c>
       <c r="F27" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G27" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1126,22 +1159,22 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D28">
-        <v>13.90299638963404</v>
+        <v>6.171394761063226</v>
       </c>
       <c r="E28" t="s">
         <v>18</v>
       </c>
       <c r="F28" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G28" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1152,19 +1185,249 @@
         <v>14</v>
       </c>
       <c r="C29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D29">
-        <v>18.85155856808055</v>
+        <v>2.020603086630215</v>
       </c>
       <c r="E29" t="s">
         <v>18</v>
       </c>
       <c r="F29" t="s">
+        <v>41</v>
+      </c>
+      <c r="G29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>14</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30">
+        <v>2.020603086630215</v>
+      </c>
+      <c r="E30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" t="s">
+        <v>41</v>
+      </c>
+      <c r="G30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>16</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31">
+        <v>1.094707468182343</v>
+      </c>
+      <c r="E31" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32">
+        <v>235.8105346386953</v>
+      </c>
+      <c r="E32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" t="s">
+        <v>43</v>
+      </c>
+      <c r="G32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33">
+        <v>67.34670428513886</v>
+      </c>
+      <c r="E33" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" t="s">
+        <v>43</v>
+      </c>
+      <c r="G33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>17</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34">
+        <v>168.4638303535564</v>
+      </c>
+      <c r="E34" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34" t="s">
+        <v>44</v>
+      </c>
+      <c r="G34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35">
+        <v>55.36382446076215</v>
+      </c>
+      <c r="E35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F35" t="s">
+        <v>45</v>
+      </c>
+      <c r="G35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>18</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36">
+        <v>54.4624139141232</v>
+      </c>
+      <c r="E36" t="s">
+        <v>21</v>
+      </c>
+      <c r="F36" t="s">
+        <v>46</v>
+      </c>
+      <c r="G36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>18</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37">
+        <v>54.4624139141232</v>
+      </c>
+      <c r="E37" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37" t="s">
+        <v>46</v>
+      </c>
+      <c r="G37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>19</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38">
+        <v>44.25783988311611</v>
+      </c>
+      <c r="E38" t="s">
+        <v>22</v>
+      </c>
+      <c r="F38" t="s">
+        <v>47</v>
+      </c>
+      <c r="G38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="1">
         <v>37</v>
       </c>
-      <c r="G29" t="s">
-        <v>40</v>
+      <c r="B39">
+        <v>20</v>
+      </c>
+      <c r="C39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39">
+        <v>10.20457403100708</v>
+      </c>
+      <c r="E39" t="s">
+        <v>22</v>
+      </c>
+      <c r="F39" t="s">
+        <v>48</v>
+      </c>
+      <c r="G39" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>